<commit_message>
Added first week for 6 month
</commit_message>
<xml_diff>
--- a/Wastes/Month 6/month_6_wastes.xlsx
+++ b/Wastes/Month 6/month_6_wastes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lunches" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
   <si>
     <t>Week</t>
   </si>
@@ -95,24 +95,6 @@
     <t>Total for 4 weeks (without debts)</t>
   </si>
   <si>
-    <t>01.06-04.06 2017</t>
-  </si>
-  <si>
-    <t>05.06-11.06 2017</t>
-  </si>
-  <si>
-    <t>12.06-18.06 2017</t>
-  </si>
-  <si>
-    <t>19.06-25.06 2017</t>
-  </si>
-  <si>
-    <t>26.06-30.06 2017</t>
-  </si>
-  <si>
-    <t>01.06-30.06 2017</t>
-  </si>
-  <si>
     <t>03.07-09.07 2017</t>
   </si>
   <si>
@@ -125,9 +107,6 @@
     <t>24.07-30.07 2017</t>
   </si>
   <si>
-    <t>(1p - печать)</t>
-  </si>
-  <si>
     <t>8p (Natasha)</t>
   </si>
   <si>
@@ -137,13 +116,25 @@
     <t>35 (Egor Rozum)</t>
   </si>
   <si>
-    <t>8p (Natasha) + 35 (Egor Rozum)</t>
-  </si>
-  <si>
     <t>16.4 (Kirill)</t>
   </si>
   <si>
     <t>11p (Olya) + 35p (Egor Rozum) + 16.4 (Kirill)</t>
+  </si>
+  <si>
+    <t>03.07-31.07 2017</t>
+  </si>
+  <si>
+    <t>31.07 2017</t>
+  </si>
+  <si>
+    <t>(1p - печать, 5p - дал девушке на маршрутку)</t>
+  </si>
+  <si>
+    <t>5p (Kirill)</t>
+  </si>
+  <si>
+    <t>8p (Natasha) + 35 (Egor Rozum) + 5(Kirill)</t>
   </si>
 </sst>
 </file>
@@ -464,7 +455,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +496,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -520,7 +511,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -530,12 +521,12 @@
       </c>
       <c r="I2">
         <f xml:space="preserve"> B2+C2+D2+E2+F2+G2+H2</f>
-        <v>7.7</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -565,7 +556,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -595,7 +586,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -624,8 +615,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
+      <c r="A6" t="s">
+        <v>33</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -659,7 +650,7 @@
       </c>
       <c r="I7">
         <f xml:space="preserve"> $I$2+$I$3+$I$4+$I$5+$I$6</f>
-        <v>7.7</v>
+        <v>13.7</v>
       </c>
     </row>
   </sheetData>
@@ -671,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,23 +713,23 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
         <f xml:space="preserve"> B2+C2+D2+E2+F2+G2+H2</f>
-        <v>0</v>
+        <v>33.4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -833,7 +824,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -867,7 +858,7 @@
       </c>
       <c r="I7">
         <f xml:space="preserve"> $I$2+$I$3+$I$4+$I$5+$I$6</f>
-        <v>0</v>
+        <v>33.4</v>
       </c>
     </row>
   </sheetData>
@@ -879,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,13 +930,13 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="J6">
         <v>62.4</v>
@@ -968,7 +959,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1022,16 +1013,19 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" t="s">
         <v>36</v>
       </c>
-      <c r="I17" t="s">
-        <v>37</v>
-      </c>
       <c r="J17">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1051,7 +1045,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1060,7 +1054,7 @@
       </c>
       <c r="J22">
         <f>$J$17+$J$18+$J$19+$J$20+$J$21</f>
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1083,7 +1077,7 @@
       </c>
       <c r="C25">
         <f xml:space="preserve"> J22</f>
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -1092,7 +1086,7 @@
       </c>
       <c r="C26">
         <f xml:space="preserve"> C24-C25</f>
-        <v>19.399999999999999</v>
+        <v>14.399999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1099,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1261,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1314,7 +1308,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,17 +1368,17 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
         <f xml:space="preserve"> B2+C2+D2+E2+F2+G2+H2</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1479,7 +1473,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1513,7 +1507,7 @@
       </c>
       <c r="I7">
         <f xml:space="preserve"> $I$2+$I$3+$I$4+$I$5+$I$6</f>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1526,7 +1520,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,7 +1530,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1545,7 +1539,7 @@
       </c>
       <c r="B2">
         <f>Lunches!I7</f>
-        <v>7.7</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1554,7 +1548,7 @@
       </c>
       <c r="B3">
         <f xml:space="preserve"> Shops!I7</f>
-        <v>0</v>
+        <v>33.4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1563,7 +1557,7 @@
       </c>
       <c r="B4">
         <f xml:space="preserve"> Debts!C26</f>
-        <v>19.399999999999999</v>
+        <v>14.399999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1581,7 +1575,7 @@
       </c>
       <c r="B6">
         <f xml:space="preserve"> Other!I7</f>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1590,7 +1584,7 @@
       </c>
       <c r="B7">
         <f xml:space="preserve"> B2+B3+B5+B6</f>
-        <v>8.6999999999999993</v>
+        <v>53.099999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>